<commit_message>
agrego inicio, cambio todo al archivo data base
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -506,44 +506,44 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09935038710</t>
+          <t>09918148311</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ora Reaver</t>
+          <t>Ben Dale</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>000022</t>
+          <t>000024</t>
         </is>
       </c>
       <c r="F2" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2" t="n">
+        <v>98720111</v>
+      </c>
+      <c r="H2" t="n">
+        <v>24680027.75</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>4</v>
       </c>
-      <c r="G2" t="n">
-        <v>88113</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8811</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>141701</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
         <v>3</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>132735</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -557,27 +557,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09928779440</t>
+          <t>09925747402</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Danielle Cabrera</t>
+          <t>Charles Simon</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>000034</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G3" t="n">
-        <v>5072010</v>
+        <v>84620631</v>
       </c>
       <c r="H3" t="n">
-        <v>507201</v>
+        <v>21155157.75</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -586,15 +586,15 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>131752</t>
+          <t>161003</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -608,27 +608,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0112025028921</t>
+          <t>0113326467515</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Debra Kenney</t>
+          <t>James Mayes</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>000010</t>
+          <t>000008</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G4" t="n">
-        <v>735923</v>
+        <v>150117</v>
       </c>
       <c r="H4" t="n">
-        <v>147185</v>
+        <v>37529.25</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -641,11 +641,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>131742</t>
+          <t>131714</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -659,44 +659,44 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0113317832746</t>
+          <t>0112026697690</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Philip Barger</t>
+          <t>Martin Devenport</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>000005</t>
+          <t>000016</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>436553</v>
+        <v>3607734</v>
       </c>
       <c r="H5" t="n">
-        <v>87311</v>
+        <v>360773</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>131708</t>
+          <t>131742</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -705,32 +705,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0113013453302</t>
+          <t>09924047189</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>John Courtright</t>
+          <t>Loraine Davis</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>000003</t>
+          <t>000004</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G6" t="n">
-        <v>358573</v>
+        <v>25737151</v>
       </c>
       <c r="H6" t="n">
-        <v>35857</v>
+        <v>2573715</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -739,11 +739,11 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>13712</t>
+          <t>131718</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -756,45 +756,45 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0112717292595</t>
+          <t>09926769398</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Christopher Currie</t>
+          <t>Brian Hatch</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>000003</t>
+          <t>000012</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" t="n">
-        <v>205457</v>
+        <v>61079939</v>
       </c>
       <c r="H7" t="n">
-        <v>51364.25</v>
+        <v>15269984.75</v>
       </c>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>13712</t>
+          <t>131742</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -812,27 +812,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>09929553446</t>
+          <t>09942396511</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Bertha Pepe</t>
+          <t>Hazel Holston</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>000006</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G8" t="n">
-        <v>776666</v>
+        <v>138712</v>
       </c>
       <c r="H8" t="n">
-        <v>155333</v>
+        <v>34678</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -845,11 +845,11 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>131711</t>
+          <t>161003</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -858,35 +858,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0112721404354</t>
+          <t>09929963778</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Latisha Reasoner</t>
+          <t>Patrick Jones</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>000009</t>
+          <t>000026</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>4038802</v>
+        <v>28485612</v>
       </c>
       <c r="H9" t="n">
-        <v>403880</v>
+        <v>2848561</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -896,7 +896,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>131731</t>
+          <t>171131</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -914,44 +914,44 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0113026767226</t>
+          <t>0112732843329</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Nicole Martin</t>
+          <t>Mona Yazzie</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>000007</t>
+          <t>000028</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G10" t="n">
-        <v>2972995</v>
+        <v>629690</v>
       </c>
       <c r="H10" t="n">
-        <v>297300</v>
+        <v>125938</v>
       </c>
       <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>3</v>
-      </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>131713</t>
+          <t>721735</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -965,40 +965,40 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>09917594806</t>
+          <t>09940926002</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Judy Caplinger</t>
+          <t>Tina Griffin</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>000013</t>
+          <t>000003</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G11" t="n">
-        <v>708942</v>
+        <v>1025936</v>
       </c>
       <c r="H11" t="n">
-        <v>141788</v>
+        <v>205187</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>131742</t>
+          <t>13712</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -1011,32 +1011,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>09935045814</t>
+          <t>0112034069516</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Kaitlin Berry</t>
+          <t>Pauline Moreland</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>000004</t>
+          <t>000033</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>121624</v>
+        <v>110028</v>
       </c>
       <c r="H12" t="n">
-        <v>30406</v>
+        <v>27507</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>131718</t>
+          <t>131744</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -1062,45 +1062,45 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0113026845845</t>
+          <t>09934630749</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Louise Solomon</t>
+          <t>Samuel Mcmurray</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>000037</t>
+          <t>000007</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G13" t="n">
-        <v>197829</v>
+        <v>52433171</v>
       </c>
       <c r="H13" t="n">
-        <v>49457.25</v>
+        <v>13108292.75</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>131792</t>
+          <t>131713</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -1118,44 +1118,44 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0112713778270</t>
+          <t>0112743371924</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Andy Hirsch</t>
+          <t>Kathy Valdez</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>000016</t>
+          <t>000022</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G14" t="n">
-        <v>47986396</v>
+        <v>536587</v>
       </c>
       <c r="H14" t="n">
-        <v>11996599</v>
+        <v>107317</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>131742</t>
+          <t>132735</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1164,49 +1164,49 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>09918389379</t>
+          <t>0112731064874</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Lillie Kiley</t>
+          <t>Javier Knight</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>000009</t>
+          <t>000018</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>20</v>
       </c>
       <c r="G15" t="n">
-        <v>230176985</v>
+        <v>88483</v>
       </c>
       <c r="H15" t="n">
-        <v>46035397</v>
+        <v>8848</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
         <v>4</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>131731</t>
+          <t>131741</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1215,32 +1215,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0113313929874</t>
+          <t>09928830626</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Yang Smith</t>
+          <t>Fred Legere</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>000018</t>
+          <t>000020</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G16" t="n">
-        <v>1469128</v>
+        <v>55510</v>
       </c>
       <c r="H16" t="n">
-        <v>293826</v>
+        <v>5551</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -1249,15 +1249,15 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>131741</t>
+          <t>131736</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1271,44 +1271,44 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>09943238335</t>
+          <t>09929098649</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>David Donatich</t>
+          <t>Rhoda Gaona</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>000009</t>
+          <t>000037</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G17" t="n">
-        <v>334149576</v>
+        <v>93571</v>
       </c>
       <c r="H17" t="n">
-        <v>66829915</v>
+        <v>9357</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
         <v>4</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>131731</t>
+          <t>131792</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1322,44 +1322,44 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>09917400302</t>
+          <t>09925901816</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>John Hammer</t>
+          <t>Millie Greco</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>000012</t>
+          <t>000024</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G18" t="n">
-        <v>39813958</v>
+        <v>1546230</v>
       </c>
       <c r="H18" t="n">
-        <v>9953489.5</v>
+        <v>309246</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>131742</t>
+          <t>141701</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1368,38 +1368,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>09912439394</t>
+          <t>0113343427879</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Nikole Stogner</t>
+          <t>Toni Caudle</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>000013</t>
+          <t>000012</t>
         </is>
       </c>
       <c r="F19" t="n">
         <v>27</v>
       </c>
       <c r="G19" t="n">
-        <v>486628014</v>
+        <v>99771</v>
       </c>
       <c r="H19" t="n">
-        <v>97325603</v>
+        <v>9977</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>4</v>
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1424,44 +1424,44 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>09921126837</t>
+          <t>09938804520</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Ricky Groves</t>
+          <t>Peggy Baker</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>000009</t>
+          <t>000033</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G20" t="n">
-        <v>62020</v>
+        <v>76284235</v>
       </c>
       <c r="H20" t="n">
-        <v>6202</v>
+        <v>19071058.75</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>131731</t>
+          <t>131744</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1475,44 +1475,44 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>09929788195</t>
+          <t>09923568419</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Rosemary Schleicher</t>
+          <t>Michael Thompson</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>000028</t>
+          <t>000007</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G21" t="n">
-        <v>24324543</v>
+        <v>210670</v>
       </c>
       <c r="H21" t="n">
-        <v>2432454</v>
+        <v>52667.5</v>
       </c>
       <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
         <v>2</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>4</v>
-      </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>721735</t>
+          <t>131713</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -1521,49 +1521,49 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>09936780943</t>
+          <t>0113326807054</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Boyce Brashear</t>
+          <t>John Betancourt</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>000020</t>
+          <t>000034</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G22" t="n">
-        <v>414940789</v>
+        <v>97651</v>
       </c>
       <c r="H22" t="n">
-        <v>82988158</v>
+        <v>9765</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>131736</t>
+          <t>131752</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1577,40 +1577,40 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0112042279236</t>
+          <t>0112026989508</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Margaret Wagner</t>
+          <t>Matthew Moore</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>000006</t>
+          <t>000015</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G23" t="n">
-        <v>87835</v>
+        <v>6146630</v>
       </c>
       <c r="H23" t="n">
-        <v>8784</v>
+        <v>614663</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>131711</t>
+          <t>131742</t>
         </is>
       </c>
       <c r="M23" t="n">
@@ -1623,32 +1623,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0113039100108</t>
+          <t>09918576604</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>James Frederick</t>
+          <t>Rochelle Longshore</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>000025</t>
+          <t>000017</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G24" t="n">
-        <v>928273</v>
+        <v>136765</v>
       </c>
       <c r="H24" t="n">
-        <v>185655</v>
+        <v>34191.25</v>
       </c>
       <c r="I24" t="n">
         <v>2</v>
@@ -1657,15 +1657,15 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>131742</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
         <v>3</v>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>150720</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1674,45 +1674,45 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>09920092328</t>
+          <t>0113331985857</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Patricia Simpson</t>
+          <t>Kathryn Childs</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>000036</t>
+          <t>000034</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G25" t="n">
-        <v>90707</v>
+        <v>23609153</v>
       </c>
       <c r="H25" t="n">
-        <v>9071</v>
+        <v>2360915</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>4</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>131792</t>
+          <t>131752</t>
         </is>
       </c>
       <c r="M25" t="n">
@@ -1730,40 +1730,40 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>09923539721</t>
+          <t>09940088826</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Michael Slaughenhoupt</t>
+          <t>Wanda Colvin</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>000026</t>
+          <t>000012</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G26" t="n">
-        <v>32557784</v>
+        <v>217352</v>
       </c>
       <c r="H26" t="n">
-        <v>8139446</v>
+        <v>54338</v>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
         <v>1</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>171131</t>
+          <t>131742</t>
         </is>
       </c>
       <c r="M26" t="n">
@@ -1781,44 +1781,44 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>09914243294</t>
+          <t>09925816404</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>James Hall</t>
+          <t>Monica Lawrence</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>000032</t>
+          <t>000014</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G27" t="n">
-        <v>934013</v>
+        <v>9680303</v>
       </c>
       <c r="H27" t="n">
-        <v>186803</v>
+        <v>968030</v>
       </c>
       <c r="I27" t="n">
         <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>161003</t>
+          <t>131742</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1827,49 +1827,49 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>099</t>
+          <t>011</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>09928047044</t>
+          <t>0112738866647</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Florence Tolbert</t>
+          <t>Monica Wing</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>000028</t>
+          <t>000026</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G28" t="n">
-        <v>484074928</v>
+        <v>137165</v>
       </c>
       <c r="H28" t="n">
-        <v>96814986</v>
+        <v>34291.25</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="n">
         <v>4</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>721735</t>
+          <t>171131</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1883,27 +1883,27 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0113343690226</t>
+          <t>0113023534517</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Jennifer Williamson</t>
+          <t>James Cummins</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>000013</t>
+          <t>000036</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G29" t="n">
-        <v>202431949</v>
+        <v>23394951</v>
       </c>
       <c r="H29" t="n">
-        <v>40486390</v>
+        <v>2339495</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1912,15 +1912,15 @@
         <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>131742</t>
+          <t>131792</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1934,40 +1934,40 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>09943507559</t>
+          <t>09927915659</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Donna Mondor</t>
+          <t>Imelda Welton</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>000007</t>
+          <t>000030</t>
         </is>
       </c>
       <c r="F30" t="n">
         <v>20</v>
       </c>
       <c r="G30" t="n">
-        <v>28744507</v>
+        <v>15287</v>
       </c>
       <c r="H30" t="n">
-        <v>2874451</v>
+        <v>1529</v>
       </c>
       <c r="I30" t="n">
         <v>1</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>131713</t>
+          <t>131728</t>
         </is>
       </c>
       <c r="M30" t="n">
@@ -1980,49 +1980,49 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>011</t>
+          <t>099</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0113017938190</t>
+          <t>09929207647</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>James Fernandez</t>
+          <t>Lori Lapidus</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>000006</t>
+          <t>000017</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G31" t="n">
-        <v>250659</v>
+        <v>1508929</v>
       </c>
       <c r="H31" t="n">
-        <v>62664.75</v>
+        <v>301786</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
       </c>
       <c r="K31" t="n">
+        <v>4</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>131742</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
         <v>2</v>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>131711</t>
-        </is>
-      </c>
-      <c r="M31" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>